<commit_message>
Added functionality to input via file
</commit_message>
<xml_diff>
--- a/dict.xlsx
+++ b/dict.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,900 +468,1340 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>avhengig</t>
+          <t>alvorlig</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dependent</t>
+          <t>serious</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Han er avhengig av kaffe om morgenen.</t>
+          <t>Situasjonen er alvorlig, og vi må handle raskt.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>He is dependent on coffee in the morning.</t>
+          <t>The situation is serious, and we need to act quickly.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>avslørt</t>
+          <t>angriper</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>revealed, exposed</t>
+          <t>attacker</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Hans hemmelige plan ble avslørt.</t>
+          <t>Løven angriper byttet sitt.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>His secret plan was revealed.</t>
+          <t>The lion attacks its prey.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bedrager</t>
+          <t>avhengig</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>fraudster</t>
+          <t>dependent</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Politiet arresterte bedrageren som hadde stjålet tusenvis av kroner.</t>
+          <t>Han er avhengig av kaffe om morgenen.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>The police arrested the fraudster who had stolen thousands of kroner.</t>
+          <t>He is dependent on coffee in the morning.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>benyttet</t>
+          <t>avslørt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>used</t>
+          <t>revealed, exposed</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Han benyttet anledningen til å takke alle involverte.</t>
+          <t>Hans hemmelige plan ble avslørt.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>He used the opportunity to thank everyone involved.</t>
+          <t>His secret plan was revealed.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>betydning</t>
+          <t>bedrager</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>meaning, significance</t>
+          <t>fraudster</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ordet har en dyp betydning.</t>
+          <t>Politiet arresterte bedrageren som hadde stjålet tusenvis av kroner.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>The word has a deep meaning.</t>
+          <t>The police arrested the fraudster who had stolen thousands of kroner.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>bidrag</t>
+          <t>benyttet</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>contribution</t>
+          <t>used</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hans bidrag til prosjektet var avgjørende for dets suksess.</t>
+          <t>Han benyttet anledningen til å takke alle involverte.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>His contribution to the project was crucial for its success.</t>
+          <t>He used the opportunity to thank everyone involved.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>bistand</t>
+          <t>betydning</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>assistance, aid</t>
+          <t>meaning, significance</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Vi tilbyr bistand til de som trenger det.</t>
+          <t>Ordet har en dyp betydning.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>We offer assistance to those who need it.</t>
+          <t>The word has a deep meaning.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>blant</t>
+          <t>bidrag</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>among</t>
+          <t>contribution</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Han er populær blant sine venner.</t>
+          <t>Hans bidrag til prosjektet var avgjørende for dets suksess.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>He is popular among his friends.</t>
+          <t>His contribution to the project was crucial for its success.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dekning</t>
+          <t>bistand</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>coverage</t>
+          <t>assistance, aid</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Det er dårlig dekning i dette området.</t>
+          <t>Vi tilbyr bistand til de som trenger det.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>There is poor coverage in this area.</t>
+          <t>We offer assistance to those who need it.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>distraherte</t>
+          <t>blant</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>distracted</t>
+          <t>among</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Han distraherte meg mens jeg studerte.</t>
+          <t>Han er populær blant sine venner.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>He distracted me while I was studying.</t>
+          <t>He is popular among his friends.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>dro</t>
+          <t>byttet</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>went, left</t>
+          <t>exchanged, swapped, or the prey</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Han dro til butikken for å kjøpe melk.</t>
+          <t>Han byttet sin gamle bil mot en ny.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>He went to the store to buy milk.</t>
+          <t>He exchanged his old car for a new one.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>egentlig</t>
+          <t>dekning</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>actually, really</t>
+          <t>coverage</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Han er egentlig fra Norge, men bor i Sverige.</t>
+          <t>Det er dårlig dekning i dette området.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>He is actually from Norway, but lives in Sweden.</t>
+          <t>There is poor coverage in this area.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ensomme</t>
+          <t>deretter</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>lonely</t>
+          <t>thereafter, then</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Han følte seg ensomme i den store byen.</t>
+          <t>Vi gikk hjem, og deretter så vi en film.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>He felt lonely in the big city.</t>
+          <t>We went home, and then we watched a movie.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>enten</t>
+          <t>distraherte</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>either</t>
+          <t>distracted</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Du må velge enten den røde eller den blå bilen.</t>
+          <t>Han distraherte meg mens jeg studerte.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>You have to choose either the red car or the blue car.</t>
+          <t>He distracted me while I was studying.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>erstatte</t>
+          <t>dro</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>replace</t>
+          <t>went, left</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Vi må erstatte den gamle datamaskinen med en ny.</t>
+          <t>Han dro til butikken for å kjøpe melk.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>We need to replace the old computer with a new one.</t>
+          <t>He went to the store to buy milk.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ettermælet</t>
+          <t>egentlig</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>legacy, reputation left behind</t>
+          <t>actually, really</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Hans ettermælet vil alltid bli husket for hans generøsitet.</t>
+          <t>Han er egentlig fra Norge, men bor i Sverige.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>His legacy will always be remembered for his generosity.</t>
+          <t>He is actually from Norway, but lives in Sweden.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>forbindelse</t>
+          <t>enhet</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>connection</t>
+          <t>unit</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Vi mistet forbindelsen under samtalen.</t>
+          <t>Hver enhet i bygningen har sin egen balkong.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>We lost the connection during the call.</t>
+          <t>Each unit in the building has its own balcony.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>forhandlingene</t>
+          <t>ensomme</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>the negotiations</t>
+          <t>lonely</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Forhandlingene mellom partene tok flere timer.</t>
+          <t>Han følte seg ensomme i den store byen.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>The negotiations between the parties took several hours.</t>
+          <t>He felt lonely in the big city.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>forholde</t>
+          <t>enten</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>relate, behave</t>
+          <t>either</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Han vet ikke hvordan han skal forholde seg til situasjonen.</t>
+          <t>Du må velge enten den røde eller den blå bilen.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>He doesn't know how to behave in the situation.</t>
+          <t>You have to choose either the red car or the blue car.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>fortjener</t>
+          <t>erfaring</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>deserve</t>
+          <t>experience</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Du fortjener en belønning for alt ditt harde arbeid.</t>
+          <t>Han har mye erfaring innen programmering.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>You deserve a reward for all your hard work.</t>
+          <t>He has a lot of experience in programming.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>imponert</t>
+          <t>erstatte</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>impressed</t>
+          <t>replace</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Jeg er veldig imponert over dine ferdigheter.</t>
+          <t>Vi må erstatte den gamle datamaskinen med en ny.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>I am very impressed by your skills.</t>
+          <t>We need to replace the old computer with a new one.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>kjemper</t>
+          <t>ettermælet</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>fights, struggles, or giants (depending on context)</t>
+          <t>legacy, reputation left behind</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Han kjemper mot en vanskelig sykdom.</t>
+          <t>Hans ettermælet vil alltid bli husket for hans generøsitet.</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>He is fighting against a difficult illness.</t>
+          <t>His legacy will always be remembered for his generosity.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>likevel</t>
+          <t>forbindelse</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>nevertheless, nonetheless</t>
+          <t>connection</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Han var veldig trøtt, men han gikk på jobb likevel.</t>
+          <t>Vi mistet forbindelsen under samtalen.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>He was very tired, but he went to work nevertheless.</t>
+          <t>We lost the connection during the call.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>markedsføre</t>
+          <t>forhandlingene</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>to market</t>
+          <t>the negotiations</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bedriften planlegger å markedsføre det nye produktet neste måned.</t>
+          <t>Forhandlingene mellom partene tok flere timer.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>The company plans to market the new product next month.</t>
+          <t>The negotiations between the parties took several hours.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>minner</t>
+          <t>forholde</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>memories</t>
+          <t>relate, behave</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Barndomsminnene mine er veldig kjære for meg.</t>
+          <t>Han vet ikke hvordan han skal forholde seg til situasjonen.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>My childhood memories are very dear to me.</t>
+          <t>He doesn't know how to behave in the situation.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>ond</t>
+          <t>fortjener</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>evil, wicked</t>
+          <t>deserve</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Han hadde en ond plan.</t>
+          <t>Du fortjener en belønning for alt ditt harde arbeid.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>He had an evil plan.</t>
+          <t>You deserve a reward for all your hard work.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>opplever</t>
+          <t>hvilket som helst</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>experiences</t>
+          <t>whichever, any</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Hun opplever mye glede i sitt nye jobb.</t>
+          <t>Du kan velge hvilket som helst alternativ.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>She experiences a lot of joy in her new job.</t>
+          <t>You can choose any option.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>overfladiske</t>
+          <t>imponert</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>superficial</t>
+          <t>impressed</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Mange mennesker er bare interessert i overfladiske detaljer.</t>
+          <t>Jeg er veldig imponert over dine ferdigheter.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Many people are only interested in superficial details.</t>
+          <t>I am very impressed by your skills.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>regjering</t>
+          <t>innsats</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>government</t>
+          <t>effort, contribution</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Regjeringen vil innføre nye skatteregler neste år.</t>
+          <t>Din innsats i prosjektet har vært uvurderlig.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>The government will introduce new tax rules next year.</t>
+          <t>Your contribution to the project has been invaluable.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>regning</t>
+          <t>kjedekollisjon</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>bill, calculation</t>
+          <t>pile-up, multiple vehicle collision</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Kan jeg få regningen, vær så snill?</t>
+          <t>Det var en stor kjedekollisjon på motorveien i går.</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Can I have the bill, please?</t>
+          <t>There was a big pile-up on the highway yesterday.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>rettferdighet</t>
+          <t>kjemper</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>justice</t>
+          <t>fights, struggles, or giants (depending on context)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Alle fortjener rettferdighet og like muligheter.</t>
+          <t>Han kjemper mot en vanskelig sykdom.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Everyone deserves justice and equal opportunities.</t>
+          <t>He is fighting against a difficult illness.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>spre</t>
+          <t>Klagar</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>to spread</t>
+          <t>Complains</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Han liker å spre glede blant vennene sine.</t>
+          <t>Han klagar alltid på været.</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>He likes to spread joy among his friends.</t>
+          <t>He always complains about the weather.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>svekker</t>
+          <t>krever</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>weakens</t>
+          <t>requires, demands</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Denne medisinen svekker immunforsvaret ditt.</t>
+          <t>Denne oppgaven krever mye tid.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>This medicine weakens your immune system.</t>
+          <t>This task requires a lot of time.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>syn</t>
+          <t>likevel</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>sight, vision</t>
+          <t>nevertheless, nonetheless</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hans syn er ikke like godt som det en gang var.</t>
+          <t>Han var veldig trøtt, men han gikk på jobb likevel.</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>His sight is not as good as it once was.</t>
+          <t>He was very tired, but he went to work nevertheless.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>syns</t>
+          <t>lyn</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>to be seen, to seem, to appear</t>
+          <t>lightning</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Det syns at han er glad.</t>
+          <t>Vi så lynet slå ned i treet.</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>It appears that he is happy.</t>
+          <t>We saw the lightning strike the tree.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>trist</t>
+          <t>markedsføre</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>sad</t>
+          <t>to market</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Det er trist å se deg så lei deg.</t>
+          <t>Bedriften planlegger å markedsføre det nye produktet neste måned.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>It is sad to see you so upset.</t>
+          <t>The company plans to market the new product next month.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>uansett</t>
+          <t>minner</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>regardless</t>
+          <t>memories</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Vi går ut uansett været.</t>
+          <t>Barndomsminnene mine er veldig kjære for meg.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>We are going out regardless of the weather.</t>
+          <t>My childhood memories are very dear to me.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>vegne</t>
+          <t>naturligvis</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>on behalf of</t>
+          <t>naturally, of course</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jeg snakker på vegne av hele teamet.</t>
+          <t>Naturligvis kan du låne bilen min.</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>I speak on behalf of the entire team.</t>
+          <t>Naturally, you can borrow my car.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>vekker</t>
+          <t>ond</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>alarm clock</t>
+          <t>evil, wicked</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Jeg setter vekkeren på 7 om morgenen.</t>
+          <t>Han hadde en ond plan.</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>I set the alarm clock for 7 in the morning.</t>
+          <t>He had an evil plan.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>virkelig</t>
+          <t>opplever</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>real, really, actual</t>
+          <t>experiences</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Er dette virkelig sant?</t>
+          <t>Hun opplever mye glede i sitt nye jobb.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Is this really true?</t>
+          <t>She experiences a lot of joy in her new job.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>overfladiske</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>superficial</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Mange mennesker er bare interessert i overfladiske detaljer.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Many people are only interested in superficial details.</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>oversetter</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>translator</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Han jobber som oversetter.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>He works as a translator.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>regjering</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>government</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Regjeringen vil innføre nye skatteregler neste år.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>The government will introduce new tax rules next year.</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>regning</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>bill, calculation</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Kan jeg få regningen, vær så snill?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Can I have the bill, please?</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>rettferdighet</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>justice</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Alle fortjener rettferdighet og like muligheter.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Everyone deserves justice and equal opportunities.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>skrive inn</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>write in, enter</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Kan du skrive inn navnet ditt her?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Can you write your name here?</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>spre</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>to spread</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Han liker å spre glede blant vennene sine.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>He likes to spread joy among his friends.</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>stjernerytter</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>star rider</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Han drømte om å bli en stjernerytter og reise gjennom galaksene.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>He dreamed of becoming a star rider and traveling through the galaxies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>svekker</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>weakens</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Denne medisinen svekker immunforsvaret ditt.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>This medicine weakens your immune system.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>syn</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>sight, vision</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Hans syn er ikke like godt som det en gang var.</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>His sight is not as good as it once was.</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>synes</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>to think, to seem, to appear</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Jeg synes det er en god idé.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>I think it is a good idea.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>syns</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>to be seen, to seem, to appear</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Det syns at han er glad.</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>It appears that he is happy.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>trist</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Det er trist å se deg så lei deg.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>It is sad to see you so upset.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>turneringen</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>the tournament</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Turneringen starter neste uke.</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>The tournament starts next week.</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>uansett</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>regardless</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Vi går ut uansett været.</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>We are going out regardless of the weather.</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Utfordrende</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Challenging</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Denne matteoppgaven er veldig utfordrende.</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>This math problem is very challenging.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>uvurderlig</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>invaluable</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Din støtte har vært uvurderlig for meg.</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Your support has been invaluable to me.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>vegne</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>on behalf of</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Jeg snakker på vegne av hele teamet.</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>I speak on behalf of the entire team.</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>vekker</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>alarm clock</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Jeg setter vekkeren på 7 om morgenen.</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>I set the alarm clock for 7 in the morning.</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>virkelig</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>real, really, actual</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Er dette virkelig sant?</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Is this really true?</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
           <t>årsaken</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B63" t="inlineStr">
         <is>
           <t>the reason</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C63" t="inlineStr">
         <is>
           <t>Årsaken til problemet er ikke kjent.</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>The reason for the problem is not known.</t>
         </is>

</xml_diff>